<commit_message>
Fix some broken tests, some WIP multiprocessing
</commit_message>
<xml_diff>
--- a/tests/test_data/data_with_multiplex_big_processed.xlsx
+++ b/tests/test_data/data_with_multiplex_big_processed.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>from</t>
   </si>
@@ -19,13 +19,16 @@
     <t>to</t>
   </si>
   <si>
-    <t>distances by car (km)</t>
+    <t>distance by car (km)</t>
   </si>
   <si>
-    <t>time by car (hours</t>
+    <t>time by car (hours)</t>
   </si>
   <si>
     <t>emissions (kg CO2)</t>
+  </si>
+  <si>
+    <t>transatlantic flight equivalents (flights)</t>
   </si>
   <si>
     <t>Bagshot, UK</t>
@@ -188,7 +191,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -198,25 +201,28 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -375,13 +381,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -471,19 +471,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -738,13 +738,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1048,19 +1042,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1311,7 +1305,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1319,10 +1313,10 @@
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.1719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.08594" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.0469" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.17188" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37" style="1" customWidth="1"/>
+    <col min="5" max="6" width="8.85156" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1341,13 +1335,16 @@
       <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5">
         <v>149.226</v>
@@ -1358,132 +1355,149 @@
       <c r="E2" s="5">
         <v>21.1751694</v>
       </c>
+      <c r="F2" s="6">
+        <v>0.02941</v>
+      </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="6">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="A3" t="s" s="7">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9">
         <v>334.255</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>3.51833333333333</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>47.4307845</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.066206</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s" s="7">
+      <c r="A4" t="s" s="7">
         <v>9</v>
       </c>
-      <c r="C4" s="8">
+      <c r="B4" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9">
         <v>610.341</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>6.99861111111111</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>86.60738790000001</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.122151</v>
       </c>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="A5" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9">
         <v>459.677</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>5.33527777777778</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>65.2281663</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.092459</v>
       </c>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="6">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="A6" t="s" s="7">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9">
         <v>658.351</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>7.22111111111111</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>93.4200069</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.13175</v>
       </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s" s="7">
+      <c r="A7" t="s" s="7">
         <v>12</v>
       </c>
-      <c r="C7" s="8">
+      <c r="B7" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9">
         <v>405.986</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>4.34388888888889</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>57.6094134</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.080014</v>
       </c>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="A8" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="C8" s="9">
         <v>189.467</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>2.47861111111111</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>26.8853673</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0.037342</v>
       </c>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="A9" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="C9" s="9">
         <v>184.517</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>2.5775</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>26.1829623</v>
       </c>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="F9" s="10">
+        <v>0.036366</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>